<commit_message>
Affiliation for Pedro updated
</commit_message>
<xml_diff>
--- a/Classification Draft Plan for Draft v0.4_github.xlsx
+++ b/Classification Draft Plan for Draft v0.4_github.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04_Research\Intent Based Networking\IETF\RG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\04_Research\Intent Based Networking\IETF\nmrg-ibn-intent-classification\nmrg-ibn-intent-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="150">
   <si>
     <t>Author</t>
   </si>
@@ -167,9 +167,6 @@
   </si>
   <si>
     <t>Clarify that the presented intent scopes are extendable.</t>
-  </si>
-  <si>
-    <t>Paderborn University</t>
   </si>
   <si>
     <t xml:space="preserve">Re-phrasing of text - "Thus, the goal of this document is to bring clarity to what an intent represents for different stakeholders,..."
@@ -497,6 +494,9 @@
   <si>
     <t>Separated the text "The key words "MUST", "MUST NOT", "REQUIRED", "SHALL", "SHALL NOT",   "SHOULD", "SHOULD NOT", "RECOMMENDED", "MAY", and "OPTIONAL" in this
    document are to be interpreted as described in RFC 2119 [RFC2119]." in a new section 2 named Key Words after Introduction.</t>
+  </si>
+  <si>
+    <t>Univ. Carlos III Madrid</t>
   </si>
 </sst>
 </file>
@@ -1365,7 +1365,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1488,11 +1487,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="883808464"/>
-        <c:axId val="883806832"/>
+        <c:axId val="1087864288"/>
+        <c:axId val="1087858304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="883808464"/>
+        <c:axId val="1087864288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1523,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1591,7 +1589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="883806832"/>
+        <c:crossAx val="1087858304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1599,7 +1597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="883806832"/>
+        <c:axId val="1087858304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1649,7 +1647,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1710,7 +1707,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="883808464"/>
+        <c:crossAx val="1087864288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,7 +1796,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2206,11 +2202,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="883812272"/>
-        <c:axId val="883801936"/>
+        <c:axId val="1087870272"/>
+        <c:axId val="883803568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="883812272"/>
+        <c:axId val="1087870272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2238,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2309,7 +2304,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="883801936"/>
+        <c:crossAx val="883803568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2317,7 +2312,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="883801936"/>
+        <c:axId val="883803568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2363,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2429,7 +2423,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="883812272"/>
+        <c:crossAx val="1087870272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2443,7 +2437,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2555,7 +2548,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2914,11 +2906,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="686254096"/>
-        <c:axId val="686247024"/>
+        <c:axId val="883807920"/>
+        <c:axId val="883805200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="686254096"/>
+        <c:axId val="883807920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2942,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3017,7 +3008,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686247024"/>
+        <c:crossAx val="883805200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3025,7 +3016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="686247024"/>
+        <c:axId val="883805200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3076,7 +3067,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3137,7 +3127,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="686254096"/>
+        <c:crossAx val="883807920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3151,7 +3141,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5211,8 +5200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,13 +5289,13 @@
         <v>4</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I10" s="25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J10" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5332,10 +5321,10 @@
         <v>8</v>
       </c>
       <c r="I11" s="53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5361,10 +5350,10 @@
         <v>8</v>
       </c>
       <c r="I12" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5390,10 +5379,10 @@
         <v>8</v>
       </c>
       <c r="I13" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5419,10 +5408,10 @@
         <v>8</v>
       </c>
       <c r="I14" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5448,10 +5437,10 @@
         <v>8</v>
       </c>
       <c r="I15" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5474,10 +5463,10 @@
         <v>3</v>
       </c>
       <c r="H16" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J16" s="61"/>
     </row>
@@ -5501,10 +5490,10 @@
         <v>2</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J17" s="61"/>
     </row>
@@ -5528,10 +5517,10 @@
         <v>2</v>
       </c>
       <c r="H18" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18" s="61"/>
     </row>
@@ -5583,7 +5572,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J20" s="61"/>
     </row>
@@ -5610,10 +5599,10 @@
         <v>8</v>
       </c>
       <c r="I21" s="54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5639,10 +5628,10 @@
         <v>10</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J22" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5668,10 +5657,10 @@
         <v>10</v>
       </c>
       <c r="I23" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J23" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="2:10" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5707,10 +5696,10 @@
         <v>8</v>
       </c>
       <c r="I25" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J25" s="65" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5736,10 +5725,10 @@
         <v>10</v>
       </c>
       <c r="I26" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5762,13 +5751,13 @@
         <v>2</v>
       </c>
       <c r="H27" s="34" t="s">
+        <v>78</v>
+      </c>
+      <c r="I27" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="34" t="s">
-        <v>80</v>
-      </c>
       <c r="J27" s="34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5794,10 +5783,10 @@
         <v>8</v>
       </c>
       <c r="I28" s="55" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J28" s="58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5819,7 +5808,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="E30" s="35" t="s">
         <v>18</v>
@@ -5834,10 +5823,10 @@
         <v>8</v>
       </c>
       <c r="I30" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J30" s="63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="113.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5848,10 +5837,10 @@
         <v>6</v>
       </c>
       <c r="D31" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="E31" s="35" t="s">
         <v>46</v>
-      </c>
-      <c r="E31" s="35" t="s">
-        <v>47</v>
       </c>
       <c r="F31" s="70">
         <v>1</v>
@@ -5863,10 +5852,10 @@
         <v>8</v>
       </c>
       <c r="I31" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J31" s="63" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5877,10 +5866,10 @@
         <v>6</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="E32" s="35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="70">
         <v>1</v>
@@ -5892,10 +5881,10 @@
         <v>8</v>
       </c>
       <c r="I32" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J32" s="63" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5906,10 +5895,10 @@
         <v>6</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F33" s="70">
         <v>1</v>
@@ -5921,10 +5910,10 @@
         <v>8</v>
       </c>
       <c r="I33" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J33" s="63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5935,10 +5924,10 @@
         <v>6</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="E34" s="35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F34" s="70">
         <v>1</v>
@@ -5950,10 +5939,10 @@
         <v>8</v>
       </c>
       <c r="I34" s="56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J34" s="63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="2:10" s="48" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5974,7 +5963,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="37" t="s">
         <v>24</v>
@@ -5989,10 +5978,10 @@
         <v>8</v>
       </c>
       <c r="I36" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J36" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6003,7 +5992,7 @@
         <v>7</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E37" s="37" t="s">
         <v>19</v>
@@ -6018,10 +6007,10 @@
         <v>8</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J37" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6032,7 +6021,7 @@
         <v>7</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E38" s="37" t="s">
         <v>20</v>
@@ -6047,10 +6036,10 @@
         <v>8</v>
       </c>
       <c r="I38" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J38" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6061,7 +6050,7 @@
         <v>7</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E39" s="37" t="s">
         <v>25</v>
@@ -6076,10 +6065,10 @@
         <v>8</v>
       </c>
       <c r="I39" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J39" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="2:10" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6115,10 +6104,10 @@
         <v>10</v>
       </c>
       <c r="I41" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J41" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:10" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6139,13 +6128,13 @@
         <v>11</v>
       </c>
       <c r="D43" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" s="71" t="s">
         <v>51</v>
-      </c>
-      <c r="E43" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="F43" s="71" t="s">
-        <v>52</v>
       </c>
       <c r="G43" s="71">
         <v>1</v>
@@ -6154,10 +6143,10 @@
         <v>8</v>
       </c>
       <c r="I43" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J43" s="64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6168,13 +6157,13 @@
         <v>11</v>
       </c>
       <c r="D44" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E44" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="F44" s="71" t="s">
         <v>51</v>
-      </c>
-      <c r="E44" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="F44" s="71" t="s">
-        <v>52</v>
       </c>
       <c r="G44" s="71">
         <v>1</v>
@@ -6193,13 +6182,13 @@
         <v>11</v>
       </c>
       <c r="D45" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F45" s="71" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G45" s="71">
         <v>0</v>
@@ -6208,10 +6197,10 @@
         <v>8</v>
       </c>
       <c r="I45" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J45" s="64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="2:10" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6222,7 +6211,7 @@
         <v>11</v>
       </c>
       <c r="D46" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E46" s="39" t="s">
         <v>15</v>
@@ -6237,10 +6226,10 @@
         <v>8</v>
       </c>
       <c r="I46" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J46" s="64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="2:10" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6251,7 +6240,7 @@
         <v>11</v>
       </c>
       <c r="D47" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E47" s="39" t="s">
         <v>28</v>
@@ -6266,10 +6255,10 @@
         <v>8</v>
       </c>
       <c r="I47" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J47" s="64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="48" spans="2:10" ht="127.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6280,10 +6269,10 @@
         <v>11</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E48" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F48" s="71">
         <v>1</v>
@@ -6295,10 +6284,10 @@
         <v>8</v>
       </c>
       <c r="I48" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J48" s="64" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6309,7 +6298,7 @@
         <v>11</v>
       </c>
       <c r="D49" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E49" s="39" t="s">
         <v>13</v>
@@ -6321,13 +6310,13 @@
         <v>3</v>
       </c>
       <c r="H49" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="I49" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="I49" s="40" t="s">
-        <v>80</v>
-      </c>
       <c r="J49" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6338,10 +6327,10 @@
         <v>11</v>
       </c>
       <c r="D50" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E50" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F50" s="71">
         <v>1</v>
@@ -6350,13 +6339,13 @@
         <v>3</v>
       </c>
       <c r="H50" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="I50" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="I50" s="40" t="s">
-        <v>80</v>
-      </c>
       <c r="J50" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="51" spans="2:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6367,7 +6356,7 @@
         <v>11</v>
       </c>
       <c r="D51" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E51" s="39" t="s">
         <v>12</v>
@@ -6382,10 +6371,10 @@
         <v>8</v>
       </c>
       <c r="I51" s="57" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J51" s="64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6396,10 +6385,10 @@
         <v>11</v>
       </c>
       <c r="D52" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E52" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F52" s="71">
         <v>1</v>
@@ -6408,13 +6397,13 @@
         <v>3</v>
       </c>
       <c r="H52" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="I52" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="I52" s="40" t="s">
-        <v>80</v>
-      </c>
       <c r="J52" s="40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6425,10 +6414,10 @@
         <v>11</v>
       </c>
       <c r="D53" s="41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E53" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F53" s="87" t="s">
         <v>36</v>
@@ -6440,10 +6429,10 @@
         <v>8</v>
       </c>
       <c r="I53" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J53" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="2:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -6495,21 +6484,21 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="19"/>
       <c r="E2" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="19"/>
       <c r="K2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>71</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
@@ -6521,10 +6510,10 @@
       <c r="H3" s="21"/>
       <c r="I3" s="17"/>
       <c r="K3" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -6532,10 +6521,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
@@ -6550,15 +6539,15 @@
         <v>3</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="15">
         <v>10</v>
@@ -6579,15 +6568,15 @@
         <v>3</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="15">
         <v>10</v>
@@ -6608,15 +6597,15 @@
         <v>1</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L6" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="15">
         <v>8</v>
@@ -6639,13 +6628,13 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="17">
         <v>10</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F8" s="6">
         <v>0</v>
@@ -6713,7 +6702,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="7">
         <v>10</v>
@@ -6788,7 +6777,7 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="6">
         <v>0</v>
@@ -6859,194 +6848,194 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s">
         <v>85</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="88" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
         <v>89</v>
-      </c>
-      <c r="B5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
         <v>91</v>
-      </c>
-      <c r="B6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
         <v>93</v>
-      </c>
-      <c r="B7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
         <v>95</v>
-      </c>
-      <c r="B8" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
         <v>97</v>
-      </c>
-      <c r="B9" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
         <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="88" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" t="s">
         <v>101</v>
-      </c>
-      <c r="B11" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="88" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" t="s">
         <v>103</v>
-      </c>
-      <c r="B12" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="88" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="89" t="s">
         <v>105</v>
-      </c>
-      <c r="B13" s="89" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="88" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
         <v>107</v>
-      </c>
-      <c r="B14" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="88" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" t="s">
         <v>109</v>
-      </c>
-      <c r="B15" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="88" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
         <v>111</v>
-      </c>
-      <c r="B16" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
         <v>113</v>
-      </c>
-      <c r="B17" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="88" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
         <v>115</v>
-      </c>
-      <c r="B18" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
         <v>117</v>
-      </c>
-      <c r="B19" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" t="s">
         <v>119</v>
-      </c>
-      <c r="B20" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="88" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" t="s">
         <v>121</v>
-      </c>
-      <c r="B21" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
         <v>123</v>
-      </c>
-      <c r="B22" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" t="s">
         <v>125</v>
-      </c>
-      <c r="B23" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="88" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" t="s">
         <v>127</v>
-      </c>
-      <c r="B24" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="88" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
         <v>129</v>
-      </c>
-      <c r="B25" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="88" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" t="s">
         <v>131</v>
-      </c>
-      <c r="B26" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Classification Draft Plan for Draft v0.4_github.xlsx
sunxueyuan-ct
</commit_message>
<xml_diff>
--- a/Classification Draft Plan for Draft v0.4_github.xlsx
+++ b/Classification Draft Plan for Draft v0.4_github.xlsx
@@ -1438,14 +1438,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:gapWidth val="219"/>
         <c:overlap val="100"/>
-        <c:axId val="134030848"/>
-        <c:axId val="134041600"/>
+        <c:axId val="129546880"/>
+        <c:axId val="202232576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="134030848"/>
+        <c:axId val="129546880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,14 +1519,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134041600"/>
+        <c:crossAx val="202232576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="134041600"/>
+        <c:axId val="202232576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1614,7 +1613,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="134030848"/>
+        <c:crossAx val="129546880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1656,7 +1655,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2059,13 +2058,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="133967232"/>
-        <c:axId val="133985792"/>
+        <c:axId val="130161280"/>
+        <c:axId val="130171648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133967232"/>
+        <c:axId val="130161280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2140,14 +2138,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133985792"/>
+        <c:crossAx val="130171648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133985792"/>
+        <c:axId val="130171648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2235,7 +2233,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="133967232"/>
+        <c:crossAx val="130161280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2307,7 +2305,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2669,13 +2667,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:overlap val="100"/>
-        <c:axId val="194654208"/>
-        <c:axId val="194656128"/>
+        <c:axId val="130315008"/>
+        <c:axId val="130316928"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="194654208"/>
+        <c:axId val="130315008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2750,14 +2747,14 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194656128"/>
+        <c:crossAx val="130316928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="194656128"/>
+        <c:axId val="130316928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2845,7 +2842,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="194654208"/>
+        <c:crossAx val="130315008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2917,7 +2914,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>